<commit_message>
LS SE channels working, committing all changes
</commit_message>
<xml_diff>
--- a/1 Hardware/MCP33151 Eval Board Bringup/Power Rails/Board Bringup Measurements.xlsx
+++ b/1 Hardware/MCP33151 Eval Board Bringup/Power Rails/Board Bringup Measurements.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Desktop\ecse478_honours_thesis\1 Hardware\MCP33151 Eval Board Bringup\Power Rails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F692B47-9A36-4F78-9712-BD5729CC1315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B100DE09-F2BD-490B-8C4B-A9D9617B106E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{7F6D996F-7E04-4D92-871E-4D697BCB5885}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" activeTab="1" xr2:uid="{7F6D996F-7E04-4D92-871E-4D697BCB5885}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Power rails" sheetId="1" r:id="rId1"/>
+    <sheet name="LS SE Gains" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="41">
   <si>
     <t>Measurements</t>
   </si>
@@ -120,14 +121,54 @@
   </si>
   <si>
     <t>board powered by phone charger brick</t>
+  </si>
+  <si>
+    <t>Methods</t>
+  </si>
+  <si>
+    <t>Input measured by multimeter in mV mode</t>
+  </si>
+  <si>
+    <t>Output measured by multimeter in mV or V mode</t>
+  </si>
+  <si>
+    <t>Hardware Output (V)</t>
+  </si>
+  <si>
+    <t>ADC averaged reading (V)</t>
+  </si>
+  <si>
+    <t>Hardware Gain (V/V)</t>
+  </si>
+  <si>
+    <t>Perceived Gain (V/V)</t>
+  </si>
+  <si>
+    <t>Output of ADC printed to serial terminal as well, averaged over 1000 samples measured at 50 Hz</t>
+  </si>
+  <si>
+    <t>Input (mV)</t>
+  </si>
+  <si>
+    <t>measured with FLIR</t>
+  </si>
+  <si>
+    <t>measured with OWON B35T+</t>
+  </si>
+  <si>
+    <t>clipped with J hooks</t>
+  </si>
+  <si>
+    <t>through alligator cables</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="168" formatCode="0.00000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -146,12 +187,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -166,12 +213,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -488,8 +544,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33445D28-1794-4B05-844D-C41C46B39434}">
   <dimension ref="A1:I23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -710,4 +766,148 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14A28D4-CBC6-46E5-BF8A-151B6CCFCF91}">
+  <dimension ref="A2:G9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>38.15</v>
+      </c>
+      <c r="B3" s="5">
+        <v>3.9469999999999998E-2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>3.9640000000000002E-2</v>
+      </c>
+      <c r="D3" s="6">
+        <f>B3/A3*1000</f>
+        <v>1.0346002621231978</v>
+      </c>
+      <c r="E3" s="6">
+        <f>C3/A3*1000</f>
+        <v>1.039056356487549</v>
+      </c>
+      <c r="G3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>38.15</v>
+      </c>
+      <c r="B4" s="5">
+        <v>0.38653999999999999</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0.38629000000000002</v>
+      </c>
+      <c r="D4" s="6">
+        <f>B4/A4*1000</f>
+        <v>10.132110091743121</v>
+      </c>
+      <c r="E4" s="6">
+        <f>C4/A4*1000</f>
+        <v>10.125557011795545</v>
+      </c>
+      <c r="G4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>38.15</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1.903</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1.8995899999999999</v>
+      </c>
+      <c r="D5" s="6">
+        <f>B5/A5*1000</f>
+        <v>49.882044560943648</v>
+      </c>
+      <c r="E5" s="6">
+        <f>C5/A5*1000</f>
+        <v>49.792660550458713</v>
+      </c>
+      <c r="G5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>38.15</v>
+      </c>
+      <c r="B6" s="5">
+        <v>3.8672</v>
+      </c>
+      <c r="C6" s="5">
+        <v>3.85968</v>
+      </c>
+      <c r="D6" s="6">
+        <f>B6/A6*1000</f>
+        <v>101.36828309305373</v>
+      </c>
+      <c r="E6" s="6">
+        <f>C6/A6*1000</f>
+        <v>101.17116644823066</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>38</v>
+      </c>
+      <c r="B8" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add temperature sensor code. refactor into BSP
</commit_message>
<xml_diff>
--- a/1 Hardware/MCP33151 Eval Board Bringup/Power Rails/Board Bringup Measurements.xlsx
+++ b/1 Hardware/MCP33151 Eval Board Bringup/Power Rails/Board Bringup Measurements.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jaspe\Desktop\ecse478_honours_thesis\1 Hardware\MCP33151 Eval Board Bringup\Power Rails\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713A302E-E2D8-4874-A303-7DBF385B0375}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95A7A1C5-3FE2-4088-B029-F5B0B69A9D5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2652" yWindow="2652" windowWidth="17280" windowHeight="10044" firstSheet="1" activeTab="1" xr2:uid="{7F6D996F-7E04-4D92-871E-4D697BCB5885}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" firstSheet="1" activeTab="3" xr2:uid="{7F6D996F-7E04-4D92-871E-4D697BCB5885}"/>
   </bookViews>
   <sheets>
     <sheet name="Power rails" sheetId="1" r:id="rId1"/>
@@ -76,7 +76,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="124">
   <si>
     <t>Measurements</t>
   </si>
@@ -415,6 +415,39 @@
   </si>
   <si>
     <t>redoing the test now with dc inputs. We don't have a good signal generator that can produce small voltages needed for testing the 100x gain</t>
+  </si>
+  <si>
+    <t>Before adding compensation resistors</t>
+  </si>
+  <si>
+    <t>Add 63k4</t>
+  </si>
+  <si>
+    <t>Vout-1v/v</t>
+  </si>
+  <si>
+    <t>Vout-10v/v</t>
+  </si>
+  <si>
+    <t>Vout-50v/v</t>
+  </si>
+  <si>
+    <t>Vout-100v/v</t>
+  </si>
+  <si>
+    <t>Add 48k7</t>
+  </si>
+  <si>
+    <t>Add 24k3</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>ADC reading</t>
+  </si>
+  <si>
+    <t>units</t>
   </si>
 </sst>
 </file>
@@ -3210,7 +3243,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14A28D4-CBC6-46E5-BF8A-151B6CCFCF91}">
   <dimension ref="A2:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -3934,10 +3967,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{507666E9-2125-403F-A1F7-D59C50427D35}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView zoomScale="98" workbookViewId="0">
-      <selection activeCell="F44" sqref="F44"/>
+    <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
+      <selection activeCell="J53" sqref="J53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4641,6 +4674,184 @@
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="H32" s="13"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" t="s">
+        <v>122</v>
+      </c>
+      <c r="C35" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>115</v>
+      </c>
+      <c r="B36">
+        <v>0.03</v>
+      </c>
+      <c r="C36" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>116</v>
+      </c>
+      <c r="B37">
+        <v>0.3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>117</v>
+      </c>
+      <c r="B38">
+        <v>1.49</v>
+      </c>
+      <c r="C38" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39">
+        <v>3.03</v>
+      </c>
+      <c r="C39" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>115</v>
+      </c>
+      <c r="B42">
+        <v>1.7389999999999999E-2</v>
+      </c>
+      <c r="C42" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>116</v>
+      </c>
+      <c r="B43">
+        <v>0.16353999999999999</v>
+      </c>
+      <c r="C43" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>117</v>
+      </c>
+      <c r="B44">
+        <v>0.80610999999999999</v>
+      </c>
+      <c r="C44" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>118</v>
+      </c>
+      <c r="B45">
+        <v>1.6320600000000001</v>
+      </c>
+      <c r="C45" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>115</v>
+      </c>
+      <c r="B48">
+        <v>6.1000000000000004E-3</v>
+      </c>
+      <c r="C48" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>116</v>
+      </c>
+      <c r="B49">
+        <v>5.0650000000000001E-2</v>
+      </c>
+      <c r="C49" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50">
+        <v>0.24623</v>
+      </c>
+      <c r="C50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>118</v>
+      </c>
+      <c r="B51">
+        <v>0.49886000000000003</v>
+      </c>
+      <c r="C51" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>118</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>